<commit_message>
Added further LDA/LogisticRegression/SVR Classifications
</commit_message>
<xml_diff>
--- a/src/Gabriel/Classification/Findings/Classification Results.xlsx
+++ b/src/Gabriel/Classification/Findings/Classification Results.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="SVM" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="SVR" sheetId="3" r:id="rId2"/>
+    <sheet name="LogisticRegression" sheetId="2" r:id="rId3"/>
+    <sheet name="LDA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="34">
   <si>
     <t>Accuracy</t>
   </si>
@@ -57,13 +58,67 @@
     <t>Net Total:</t>
   </si>
   <si>
-    <t>SVM Classification (Default Parameters). 60/40 Split. Lag = 0</t>
-  </si>
-  <si>
-    <t>SVM Classification (Default Parameters). 70/30 Split. Lag = 0</t>
-  </si>
-  <si>
-    <t>SVM Classification (Default Parameters). 80/20 Split. Lag = 0</t>
+    <t>SVC(C=1.0, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=3, gamma='auto', kernel='linear', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False)</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>poly</t>
+  </si>
+  <si>
+    <t>Data Normalization</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Lag Value</t>
+  </si>
+  <si>
+    <t>SVC(C=1.0, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=2, gamma='auto', kernel='poly', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False)</t>
+  </si>
+  <si>
+    <t>SVC(C=1.0, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=3, gamma='auto', kernel='sigmoid', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False)</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>SVM Classification (Default Parameters). 60/40 Split.</t>
+  </si>
+  <si>
+    <t>SVM Classification (Default Parameters). 70/30 Split.</t>
+  </si>
+  <si>
+    <t>SVM Classification (Default Parameters). 80/20 Split.</t>
+  </si>
+  <si>
+    <t>SVR Classification (Default Parameters). 80/20 Split.</t>
+  </si>
+  <si>
+    <t>SVR(C=1.0, cache_size=200, coef0=0.0, degree=3, epsilon=0.1, gamma='auto', kernel='rbf', max_iter=-1, shrinking=True, tol=0.001, verbose=False)</t>
+  </si>
+  <si>
+    <t>LogisticRegression</t>
+  </si>
+  <si>
+    <t>LogisticRegression(C=1.0, class_weight=None, dual=False, fit_intercept=True, intercept_scaling=1, max_iter=100, multi_class='ovr', n_jobs=1, penalty='l2', random_state=None, solver='liblinear', tol=0.0001, verbose=0, warm_start=False)</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>LinearDiscriminantAnalysis(n_components=None, priors=None, shrinkage=None, solver='svd', store_covariance=False, tol=0.0001)</t>
   </si>
 </sst>
 </file>
@@ -107,10 +162,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,22 +470,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="59.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="58" customWidth="1"/>
+    <col min="6" max="6" width="93.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -435,8 +497,12 @@
         <v>5</v>
       </c>
       <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -444,8 +510,12 @@
         <v>14980</v>
       </c>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -453,8 +523,12 @@
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -463,8 +537,12 @@
         <v>14976</v>
       </c>
       <c r="C4" s="2"/>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -472,88 +550,447 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
         <v>55.967284259700001</v>
       </c>
-      <c r="E7">
+      <c r="I7">
         <v>65.568683427500005</v>
       </c>
-      <c r="F7">
+      <c r="J7">
         <v>55.967284259700001</v>
       </c>
-      <c r="G7">
+      <c r="K7">
         <v>42.507127485600002</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
         <v>55.9091920766</v>
       </c>
-      <c r="E8">
+      <c r="I8">
         <v>65.865148583700005</v>
       </c>
-      <c r="F8">
+      <c r="J8">
         <v>55.9091920766</v>
       </c>
-      <c r="G8">
+      <c r="K8">
         <v>42.981193647200001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="H9">
+        <v>56.575433911899999</v>
+      </c>
+      <c r="I9">
+        <v>68.039669511499994</v>
+      </c>
+      <c r="J9">
+        <v>56.575433911899999</v>
+      </c>
+      <c r="K9">
+        <v>44.322678795000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>59.178905206899998</v>
+      </c>
+      <c r="I10">
+        <v>59.0914759948</v>
+      </c>
+      <c r="J10">
+        <v>59.178905206899998</v>
+      </c>
+      <c r="K10">
+        <v>57.362362123399997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11">
+        <v>61.281708945299997</v>
+      </c>
+      <c r="I11">
+        <v>62.0775826008</v>
+      </c>
+      <c r="J11">
+        <v>61.281708945299997</v>
+      </c>
+      <c r="K11">
+        <v>58.8278743953</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12">
+        <v>54.038718291099997</v>
+      </c>
+      <c r="I12">
+        <v>29.201830745399999</v>
+      </c>
+      <c r="J12">
+        <v>54.038718291099997</v>
+      </c>
+      <c r="K12">
+        <v>37.9149230393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>54.038718291099997</v>
+      </c>
+      <c r="I13">
+        <v>29.201830745399999</v>
+      </c>
+      <c r="J13">
+        <v>54.038718291099997</v>
+      </c>
+      <c r="K13">
+        <v>37.9149230393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>56.575433911899999</v>
-      </c>
-      <c r="E9">
-        <v>68.039669511499994</v>
-      </c>
-      <c r="F9">
-        <v>56.575433911899999</v>
-      </c>
-      <c r="G9">
-        <v>44.322678795000002</v>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>58.931552587600002</v>
+      </c>
+      <c r="I14">
+        <v>58.863086638200002</v>
+      </c>
+      <c r="J14">
+        <v>58.931552587600002</v>
+      </c>
+      <c r="K14">
+        <v>56.5737734796</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>59.499165275499998</v>
+      </c>
+      <c r="I15">
+        <v>61.0202837167</v>
+      </c>
+      <c r="J15">
+        <v>59.499165275499998</v>
+      </c>
+      <c r="K15">
+        <v>54.412707881800003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>59.385437541800002</v>
+      </c>
+      <c r="I16">
+        <v>60.881609437199998</v>
+      </c>
+      <c r="J16">
+        <v>59.385437541800002</v>
+      </c>
+      <c r="K16">
+        <v>54.716691161699998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17">
+        <v>59.151636606499999</v>
+      </c>
+      <c r="I17">
+        <v>60.054575501800002</v>
+      </c>
+      <c r="J17">
+        <v>59.151636606499999</v>
+      </c>
+      <c r="K17">
+        <v>54.853667426999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>59.185036740100003</v>
+      </c>
+      <c r="I18">
+        <v>60.592879119000003</v>
+      </c>
+      <c r="J18">
+        <v>59.185036740100003</v>
+      </c>
+      <c r="K18">
+        <v>54.7262643129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19">
+        <v>61.381842456599998</v>
+      </c>
+      <c r="I19">
+        <v>62.4629248022</v>
+      </c>
+      <c r="J19">
+        <v>61.381842456599998</v>
+      </c>
+      <c r="K19">
+        <v>58.636814438800002</v>
       </c>
     </row>
   </sheetData>
@@ -564,24 +1001,867 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>14980</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <f>(B2-B3)</f>
+        <v>14976</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>58.2109479306</v>
+      </c>
+      <c r="I7">
+        <v>68.891510136099996</v>
+      </c>
+      <c r="J7">
+        <v>58.2109479306</v>
+      </c>
+      <c r="K7">
+        <v>47.928224894800003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8">
+        <v>37.383177570100003</v>
+      </c>
+      <c r="I8">
+        <v>37.185751272899999</v>
+      </c>
+      <c r="J8">
+        <v>37.383177570100003</v>
+      </c>
+      <c r="K8">
+        <v>35.513537569599997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>59.833055091799999</v>
+      </c>
+      <c r="I9">
+        <v>60.559030404300003</v>
+      </c>
+      <c r="J9">
+        <v>59.833055091799999</v>
+      </c>
+      <c r="K9">
+        <v>56.5288131354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>61.502504173600002</v>
+      </c>
+      <c r="I10">
+        <v>61.1884179503</v>
+      </c>
+      <c r="J10">
+        <v>61.502504173600002</v>
+      </c>
+      <c r="K10">
+        <v>60.814999720000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>59.9866399466</v>
+      </c>
+      <c r="I11">
+        <v>59.700955902399997</v>
+      </c>
+      <c r="J11">
+        <v>59.9866399466</v>
+      </c>
+      <c r="K11">
+        <v>58.884446210699998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>59.719438877800002</v>
+      </c>
+      <c r="I12">
+        <v>59.406571147800001</v>
+      </c>
+      <c r="J12">
+        <v>59.719438877800002</v>
+      </c>
+      <c r="K12">
+        <v>58.383381453299997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>60.187040748199998</v>
+      </c>
+      <c r="I13">
+        <v>60.356288640199999</v>
+      </c>
+      <c r="J13">
+        <v>60.187040748199998</v>
+      </c>
+      <c r="K13">
+        <v>58.156473373300003</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>14980</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <f>(B2-B3)</f>
+        <v>14976</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7">
+        <v>59.879839786399998</v>
+      </c>
+      <c r="H7">
+        <v>60.316500231900001</v>
+      </c>
+      <c r="I7">
+        <v>59.879839786399998</v>
+      </c>
+      <c r="J7">
+        <v>57.3218150334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>60.033388981599998</v>
+      </c>
+      <c r="H8">
+        <v>60.673942109499997</v>
+      </c>
+      <c r="I8">
+        <v>60.033388981599998</v>
+      </c>
+      <c r="J8">
+        <v>56.973450939700001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9">
+        <v>60.100166944900003</v>
+      </c>
+      <c r="H9">
+        <v>62.868161630899998</v>
+      </c>
+      <c r="I9">
+        <v>60.100166944900003</v>
+      </c>
+      <c r="J9">
+        <v>54.3468630132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10">
+        <v>59.285237140900001</v>
+      </c>
+      <c r="H10">
+        <v>62.3217159501</v>
+      </c>
+      <c r="I10">
+        <v>59.285237140900001</v>
+      </c>
+      <c r="J10">
+        <v>53.071819029300002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11">
+        <v>59.6526386106</v>
+      </c>
+      <c r="H11">
+        <v>61.542743095200002</v>
+      </c>
+      <c r="I11">
+        <v>59.6526386106</v>
+      </c>
+      <c r="J11">
+        <v>54.587651135599998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12">
+        <v>58.784235136900001</v>
+      </c>
+      <c r="H12">
+        <v>61.158612925600004</v>
+      </c>
+      <c r="I12">
+        <v>58.784235136900001</v>
+      </c>
+      <c r="J12">
+        <v>52.956615678600002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>14980</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <f>(B2-B3)</f>
+        <v>14976</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>58.711615487300001</v>
+      </c>
+      <c r="G7">
+        <v>58.863439943700001</v>
+      </c>
+      <c r="H7">
+        <v>58.711615487300001</v>
+      </c>
+      <c r="I7">
+        <v>56.0233964492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>58.764607679500003</v>
+      </c>
+      <c r="G8">
+        <v>58.941840032199998</v>
+      </c>
+      <c r="H8">
+        <v>58.764607679500003</v>
+      </c>
+      <c r="I8">
+        <v>55.695219033800001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9">
+        <v>59.432387312199999</v>
+      </c>
+      <c r="G9">
+        <v>62.632523081099997</v>
+      </c>
+      <c r="H9">
+        <v>59.432387312199999</v>
+      </c>
+      <c r="I9">
+        <v>52.753529762500001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>57.448229792900001</v>
+      </c>
+      <c r="G10">
+        <v>60.7031508217</v>
+      </c>
+      <c r="H10">
+        <v>57.448229792900001</v>
+      </c>
+      <c r="I10">
+        <v>48.978434639900001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11">
+        <v>58.851035404100003</v>
+      </c>
+      <c r="G11">
+        <v>59.996409077599999</v>
+      </c>
+      <c r="H11">
+        <v>58.851035404100003</v>
+      </c>
+      <c r="I11">
+        <v>53.947670178400003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12">
+        <v>58.3834335337</v>
+      </c>
+      <c r="G12">
+        <v>61.015316604699997</v>
+      </c>
+      <c r="H12">
+        <v>58.3834335337</v>
+      </c>
+      <c r="I12">
+        <v>51.924376323399997</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>